<commit_message>
Lista de requisitos com base em Brainstorm
Lista de requisitos atualizada com base em Brainstorm
</commit_message>
<xml_diff>
--- a/PastaDocumentos/2SIPH-ListaRequisitos-SiEstacionamento.xlsx
+++ b/PastaDocumentos/2SIPH-ListaRequisitos-SiEstacionamento.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FIAP-2024\TEMP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37333D0C-DA00-4863-B846-A6DEB4D0481C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F45244-D960-432F-8BE7-BB261E2572E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{42041E6B-20B5-40F2-9291-CD50E6A1A57E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="53">
   <si>
     <t>Lista de requisitos</t>
   </si>
@@ -100,6 +100,90 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Terminal mobile de atendimento;</t>
+  </si>
+  <si>
+    <t>Sensor de vagas livres/ocupadas</t>
+  </si>
+  <si>
+    <t>Controle de filas de entrada e saída</t>
+  </si>
+  <si>
+    <t>Controle de tickets</t>
+  </si>
+  <si>
+    <t>Tratamento de meios de pagamento</t>
+  </si>
+  <si>
+    <t>Tipificação de uso (mensalista/avulso/conveniado)</t>
+  </si>
+  <si>
+    <t>Administração de caixa</t>
+  </si>
+  <si>
+    <t>Configuração de tabelas preços (dias/horários/tipo de uso)</t>
+  </si>
+  <si>
+    <t>Emissão de nota fiscal</t>
+  </si>
+  <si>
+    <t>Gestão de cobranças de mensalistas e conveniados</t>
+  </si>
+  <si>
+    <t>Reconhecimento de placa para recuperar dados cadastrais</t>
+  </si>
+  <si>
+    <t>Cadastro de veículos e clientes</t>
+  </si>
+  <si>
+    <t>Reservar vagas</t>
+  </si>
+  <si>
+    <t>Solução mobile para o cliente fazer reservas e pagamentos</t>
+  </si>
+  <si>
+    <t>Orientação por voz</t>
+  </si>
+  <si>
+    <t>Integração com TAG</t>
+  </si>
+  <si>
+    <t>Relatório de gerenciamento de média de ocupação de vagas por dia e horário</t>
+  </si>
+  <si>
+    <t>Relatório de gerenciamento do valor recebido por meio de pagamento por mês</t>
+  </si>
+  <si>
+    <t>Forum/Sistema de Denuncias</t>
+  </si>
+  <si>
+    <t>Estacionamento Vertical com elevador</t>
+  </si>
+  <si>
+    <t>Planta digital</t>
+  </si>
+  <si>
+    <t>Sistema de fidelidade</t>
+  </si>
+  <si>
+    <t>Controle do período estacionado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sistema de vigilância automatizado, com câmeras inteligentes. </t>
+  </si>
+  <si>
+    <t>Ticket digital via e-mail ou sms</t>
+  </si>
+  <si>
+    <t>Sistema de Segurança contra roubos </t>
+  </si>
+  <si>
+    <t>Sistema de redirecionamento para o condutor indicando vagas livres</t>
+  </si>
+  <si>
+    <t>Mostrar quantidade de vagas disponíveis em determinado local</t>
   </si>
 </sst>
 </file>
@@ -202,7 +286,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -226,9 +310,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -543,19 +624,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2924E7E3-4BB6-4F36-B430-910D22753DB0}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="68.85546875" customWidth="1"/>
+    <col min="1" max="1" width="74.7109375" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" customWidth="1"/>
     <col min="3" max="3" width="14.5703125" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" customWidth="1"/>
-    <col min="5" max="5" width="92.28515625" customWidth="1"/>
+    <col min="5" max="5" width="86.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -711,315 +792,258 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
+      <c r="A13" s="11" t="s">
+        <v>25</v>
+      </c>
       <c r="B13" s="12"/>
       <c r="C13" s="13"/>
       <c r="D13" s="14"/>
       <c r="E13" s="15"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
+      <c r="A14" s="16" t="s">
+        <v>26</v>
+      </c>
       <c r="B14" s="12"/>
       <c r="C14" s="13"/>
       <c r="D14" s="14"/>
       <c r="E14" s="15"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
+      <c r="A15" s="16" t="s">
+        <v>27</v>
+      </c>
       <c r="B15" s="12"/>
       <c r="C15" s="13"/>
       <c r="D15" s="14"/>
       <c r="E15" s="15"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
+      <c r="A16" s="16" t="s">
+        <v>28</v>
+      </c>
       <c r="B16" s="12"/>
       <c r="C16" s="13"/>
       <c r="D16" s="14"/>
       <c r="E16" s="15"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
+      <c r="A17" s="16" t="s">
+        <v>29</v>
+      </c>
       <c r="B17" s="12"/>
       <c r="C17" s="13"/>
       <c r="D17" s="14"/>
       <c r="E17" s="15"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="16"/>
+      <c r="A18" s="16" t="s">
+        <v>30</v>
+      </c>
       <c r="B18" s="12"/>
       <c r="C18" s="13"/>
       <c r="D18" s="14"/>
       <c r="E18" s="15"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
+      <c r="A19" s="16" t="s">
+        <v>31</v>
+      </c>
       <c r="B19" s="12"/>
       <c r="C19" s="13"/>
       <c r="D19" s="14"/>
       <c r="E19" s="15"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
+        <v>32</v>
+      </c>
       <c r="B20" s="12"/>
       <c r="C20" s="13"/>
       <c r="D20" s="14"/>
       <c r="E20" s="15"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="16"/>
+      <c r="A21" s="16" t="s">
+        <v>33</v>
+      </c>
       <c r="B21" s="12"/>
       <c r="C21" s="13"/>
       <c r="D21" s="14"/>
       <c r="E21" s="15"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="16"/>
+      <c r="A22" s="16" t="s">
+        <v>34</v>
+      </c>
       <c r="B22" s="12"/>
       <c r="C22" s="13"/>
       <c r="D22" s="14"/>
       <c r="E22" s="15"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="16"/>
+      <c r="A23" s="16" t="s">
+        <v>35</v>
+      </c>
       <c r="B23" s="12"/>
       <c r="C23" s="13"/>
       <c r="D23" s="14"/>
       <c r="E23" s="15"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="16"/>
+      <c r="A24" s="16" t="s">
+        <v>36</v>
+      </c>
       <c r="B24" s="12"/>
       <c r="C24" s="13"/>
       <c r="D24" s="14"/>
       <c r="E24" s="15"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="16"/>
+      <c r="A25" s="16" t="s">
+        <v>37</v>
+      </c>
       <c r="B25" s="12"/>
       <c r="C25" s="13"/>
       <c r="D25" s="14"/>
       <c r="E25" s="15"/>
     </row>
-    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="6"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="10"/>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="12"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="15"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="12"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="15"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="12"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="15"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="12"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="15"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" s="12"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="15"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="12"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="15"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="12"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="15"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" s="12"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="15"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" s="12"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="15"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35" s="12"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="15"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B36" s="12"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="15"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37" s="12"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="15"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B38" s="12"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="15"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B39" s="12"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="15"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B40" s="12"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100223DA578DE33E44E8DD11C312C11F0C0" ma:contentTypeVersion="11" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="1f1bf57ebb3445789c15eebb8f8f3867">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7bc641a7-997f-4048-a412-d593c6319208" xmlns:ns3="7e3d2bc7-1e8b-4412-b9e4-2111d76bd9c9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c426eb50fe407b082a13f745c724ecdb" ns2:_="" ns3:_="">
-    <xsd:import namespace="7bc641a7-997f-4048-a412-d593c6319208"/>
-    <xsd:import namespace="7e3d2bc7-1e8b-4412-b9e4-2111d76bd9c9"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
-                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="7bc641a7-997f-4048-a412-d593c6319208" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="9" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Marcações de imagem" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="e2398b20-2c76-408b-9565-673d41e5947a" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="MediaServiceMetadata" ma:index="11" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="12" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceSearchProperties" ma:index="13" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="14" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="15" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="18" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="7e3d2bc7-1e8b-4412-b9e4-2111d76bd9c9" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="TaxCatchAll" ma:index="10" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{f0f23bec-50ac-47da-84b3-e98b71cf663a}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="7e3d2bc7-1e8b-4412-b9e4-2111d76bd9c9">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de Conteúdo"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCE55239-3B84-4C7D-85A8-1299C75BC4A3}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F9836474-5EE6-4417-B4D0-222B651917AA}"/>
 </file>
</xml_diff>